<commit_message>
adds the K-Means data
</commit_message>
<xml_diff>
--- a/latex tables/forestFiresRegression_excel.xlsx
+++ b/latex tables/forestFiresRegression_excel.xlsx
@@ -1,19 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr date1904="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nardi\Documents\2019-2020 School Year\Fall Semester\CSCI 447\CSCI447_knn_assignment\latex tables\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66ADF58F-EB1E-42A7-B84B-D2895C99B680}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Export Summary" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet 1" sheetId="2" r:id="rId5"/>
+    <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -76,15 +92,29 @@
   </si>
   <si>
     <t>K=44</t>
+  </si>
+  <si>
+    <t>Kmeans</t>
+  </si>
+  <si>
+    <t>K=22</t>
+  </si>
+  <si>
+    <t>KMeans</t>
+  </si>
+  <si>
+    <t>K=28</t>
+  </si>
+  <si>
+    <t>K=30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="0.000000"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -103,13 +133,13 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="12"/>
       <color indexed="11"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -262,67 +292,70 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -332,29 +365,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="015e88b1"/>
-      <rgbColor rgb="01eef3f4"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="015E88B1"/>
+      <rgbColor rgb="01EEF3F4"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -553,7 +642,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -572,7 +661,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -602,7 +691,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -628,7 +717,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -654,7 +743,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -680,7 +769,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -706,7 +795,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -732,7 +821,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -758,7 +847,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -784,7 +873,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -810,7 +899,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -823,9 +912,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -842,7 +937,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -861,7 +956,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -887,7 +982,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -913,7 +1008,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -939,7 +1034,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -965,7 +1060,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -991,7 +1086,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1017,7 +1112,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1043,7 +1138,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1069,7 +1164,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1095,7 +1190,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1108,9 +1203,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1124,7 +1225,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1143,7 +1244,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1173,7 +1274,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1199,7 +1300,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1225,7 +1326,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1251,7 +1352,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1277,7 +1378,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1303,7 +1404,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1329,7 +1430,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1355,7 +1456,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1381,7 +1482,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1394,58 +1495,68 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="4" width="33.6016" customWidth="1"/>
+    <col min="2" max="4" width="33.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="50" customHeight="1">
-      <c r="B3" t="s" s="1">
+    <row r="3" spans="2:4" ht="49.95" customHeight="1">
+      <c r="B3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
     </row>
-    <row r="7">
-      <c r="B7" t="s" s="2">
+    <row r="7" spans="2:4" ht="17.399999999999999">
+      <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9">
-      <c r="B9" t="s" s="3">
+    <row r="9" spans="2:4" ht="15">
+      <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
     </row>
-    <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
+    <row r="10" spans="2:4" ht="15">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="5">
+      <c r="D10" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1454,196 +1565,268 @@
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D10" location="'Sheet 1'!R2C1" tooltip="" display="Sheet 1"/>
+    <hyperlink ref="D10" location="'Sheet 1'!R2C1" display="Sheet 1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:F8"/>
+  <dimension ref="A1:IV11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="19.95" customHeight="1"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="6" customWidth="1"/>
-    <col min="7" max="256" width="16.3516" style="6" customWidth="1"/>
+    <col min="1" max="256" width="16.33203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="7">
+    <row r="1" spans="1:6" ht="27.6" customHeight="1">
+      <c r="A1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
-    <row r="2" ht="44.25" customHeight="1">
-      <c r="A2" t="s" s="8">
+    <row r="2" spans="1:6" ht="44.25" customHeight="1">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s" s="8">
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s" s="8">
+      <c r="C2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s" s="8">
+      <c r="D2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s" s="8">
+      <c r="E2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s" s="8">
+      <c r="F2" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="9">
+    <row r="3" spans="1:6" ht="20.25" customHeight="1">
+      <c r="A3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="10">
+        <v>4176.5423449999998</v>
+      </c>
+      <c r="E3" s="10">
+        <f>SQRT(D3)</f>
+        <v>64.626173838468887</v>
+      </c>
+      <c r="F3" s="11">
+        <f>E3/63.655818</f>
+        <v>1.0152437886898082</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="15">
+        <v>4174.9863519999999</v>
+      </c>
+      <c r="E4" s="15">
+        <f>SQRT(D4)</f>
+        <v>64.614134305119336</v>
+      </c>
+      <c r="F4" s="16">
+        <f>E4/63.655818</f>
+        <v>1.0150546538435707</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A5" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="15">
+        <v>4178.4562120000001</v>
+      </c>
+      <c r="E5" s="15">
+        <f>SQRT(D5)</f>
+        <v>64.640979355204692</v>
+      </c>
+      <c r="F5" s="16">
+        <f>E5/63.655818</f>
+        <v>1.0154763757054335</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s" s="10">
+      <c r="B6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s" s="11">
+      <c r="C6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D6" s="15">
         <v>3682.563545</v>
       </c>
-      <c r="E3" s="12">
-        <f>SQRT(D3)</f>
-        <v>60.68412926787366</v>
-      </c>
-      <c r="F3" s="13">
-        <f>E3/63.655818</f>
-        <v>0.9533163059482428</v>
+      <c r="E6" s="15">
+        <f>SQRT(D6)</f>
+        <v>60.684129267873658</v>
+      </c>
+      <c r="F6" s="16">
+        <f>E6/63.655818</f>
+        <v>0.95331630594824279</v>
       </c>
     </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="14">
+    <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s" s="15">
+      <c r="B7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s" s="16">
+      <c r="C7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D7" s="15">
         <v>3706.201716</v>
       </c>
-      <c r="E4" s="17">
-        <f>SQRT(D4)</f>
-        <v>60.87858175089167</v>
-      </c>
-      <c r="F4" s="18">
-        <f>E4/63.655818</f>
+      <c r="E7" s="15">
+        <f>SQRT(D7)</f>
+        <v>60.878581750891669</v>
+      </c>
+      <c r="F7" s="16">
+        <f>E7/63.655818</f>
         <v>0.9563710539528637</v>
       </c>
     </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="14">
+    <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s" s="15">
+      <c r="B8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s" s="16">
+      <c r="C8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="17">
-        <v>3875.457522</v>
-      </c>
-      <c r="E5" s="17">
-        <f>SQRT(D5)</f>
+      <c r="D8" s="15">
+        <v>3875.4575220000002</v>
+      </c>
+      <c r="E8" s="15">
+        <f>SQRT(D8)</f>
         <v>62.25317278661386</v>
       </c>
-      <c r="F5" s="18">
-        <f>E5/63.655818</f>
-        <v>0.977965168660842</v>
+      <c r="F8" s="16">
+        <f>E8/63.655818</f>
+        <v>0.97796516866084204</v>
       </c>
     </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="14">
+    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s" s="15">
+      <c r="B9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s" s="16">
+      <c r="C9" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="17">
-        <v>4185.986305</v>
-      </c>
-      <c r="E6" s="17">
-        <f>SQRT(D6)</f>
-        <v>64.69919864264163</v>
-      </c>
-      <c r="F6" s="18">
-        <f>E6/63.655818</f>
-        <v>1.016390970620182</v>
+      <c r="D9" s="15">
+        <v>4185.9863050000004</v>
+      </c>
+      <c r="E9" s="15">
+        <f>SQRT(D9)</f>
+        <v>64.699198642641633</v>
+      </c>
+      <c r="F9" s="16">
+        <f>E9/63.655818</f>
+        <v>1.0163909706201817</v>
       </c>
     </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="14">
+    <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s" s="15">
+      <c r="B10" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s" s="16">
+      <c r="C10" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="17">
-        <v>4187.302436</v>
-      </c>
-      <c r="E7" s="17">
-        <f>SQRT(D7)</f>
-        <v>64.709368997078</v>
-      </c>
-      <c r="F7" s="18">
-        <f>E7/63.655818</f>
-        <v>1.016550741631786</v>
+      <c r="D10" s="15">
+        <v>4187.3024359999999</v>
+      </c>
+      <c r="E10" s="15">
+        <f>SQRT(D10)</f>
+        <v>64.709368997078002</v>
+      </c>
+      <c r="F10" s="16">
+        <f>E10/63.655818</f>
+        <v>1.0165507416317863</v>
       </c>
     </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="14">
+    <row r="11" spans="1:6" ht="19.95" customHeight="1">
+      <c r="A11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s" s="15">
+      <c r="B11" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s" s="16">
+      <c r="C11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D11" s="15">
         <v>4189.678148</v>
       </c>
-      <c r="E8" s="17">
-        <f>SQRT(D8)</f>
-        <v>64.7277231794847</v>
-      </c>
-      <c r="F8" s="18">
-        <f>E8/63.655818</f>
-        <v>1.016839076350958</v>
+      <c r="E11" s="15">
+        <f>SQRT(D11)</f>
+        <v>64.727723179484698</v>
+      </c>
+      <c r="F11" s="16">
+        <f>E11/63.655818</f>
+        <v>1.0168390763509583</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F11">
+    <sortCondition ref="A3"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>